<commit_message>
problem 2 fix bug
</commit_message>
<xml_diff>
--- a/2_tra_cluster/data/beijing_20200_traj_cluster.xlsx
+++ b/2_tra_cluster/data/beijing_20200_traj_cluster.xlsx
@@ -440,727 +440,727 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>